<commit_message>
Fix the calculation issue of the Milestone class.
</commit_message>
<xml_diff>
--- a/tests/files/happy_path_sorted.xlsx
+++ b/tests/files/happy_path_sorted.xlsx
@@ -614,42 +614,42 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Andy Wu</t>
+          <t>Sharry Xu</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Review the design</t>
+          <t>Develop Jira tool</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://jira.com/browse/proj-002</t>
+          <t>https://jira.com/browse/proj-001</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>M110</t>
+          <t>M109</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
           <t>High</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -664,7 +664,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -679,7 +679,7 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
@@ -706,22 +706,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Tony Wei</t>
+          <t>Andy Wu</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Sign Off</t>
+          <t>Review the design</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://jira.com/browse/proj-005</t>
+          <t>https://jira.com/browse/proj-002</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>R135 S2</t>
+          <t>M110</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -741,7 +741,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Middle</t>
+          <t>High</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -890,42 +890,42 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Sharry Xu</t>
+          <t>Tony Wei</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Develop Jira tool</t>
+          <t>Sign Off</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://jira.com/browse/proj-001</t>
+          <t>https://jira.com/browse/proj-005</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>M109</t>
+          <t>R135 S2</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>High</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Middle</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -940,7 +940,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Critical</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -955,7 +955,7 @@
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">

</xml_diff>